<commit_message>
Allow user to select level of aggregation
</commit_message>
<xml_diff>
--- a/reference/dictionaries/MT.xlsx
+++ b/reference/dictionaries/MT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.humphreys\Documents\Development\EHR-BSI-TryingHarmonisedExcel\reference\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F57F634-1223-4B4C-87CF-BE2610D6C36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF6864C-9D61-44A5-B54E-A4EFE7B74487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
@@ -2649,7 +2649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -3777,9 +3777,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="21.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>